<commit_message>
Update to Weekly Sprint
</commit_message>
<xml_diff>
--- a/Documentation/Scrum_Journal_202.xlsx
+++ b/Documentation/Scrum_Journal_202.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10410"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mounicakandi/Desktop/202/team-project-incognito/Documentation/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4C9CA87-56CF-3C4E-869D-9EA3B509E296}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="13440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="28800" windowHeight="13440"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104">
   <si>
     <t>WEEK 1 ( FEB 27 - MARCH 5)</t>
   </si>
@@ -85,34 +79,55 @@
     <t>XP Core Value</t>
   </si>
   <si>
+    <t>1. Courage</t>
+  </si>
+  <si>
+    <t>We needed courage to take up the task and implement all out task on time.</t>
+  </si>
+  <si>
+    <t>2. Comunication</t>
+  </si>
+  <si>
+    <t>We followed Communication during this Weekly Scrum since it is necessary to update everybody about our work</t>
+  </si>
+  <si>
+    <t>3. Respect</t>
+  </si>
+  <si>
+    <t>It is necessary to Respect others opinion and time to keep every team member focused on the work.</t>
+  </si>
+  <si>
+    <t>WEEK 2 ( MARCH 6 - MARCH 12)</t>
+  </si>
+  <si>
+    <t>Was the scrum master for this sprint. Meanwhile also worked on the frontend decisions along with the tables</t>
+  </si>
+  <si>
+    <t>Design frontent booking route component</t>
+  </si>
+  <si>
+    <t>Finalized the table structure for the Database</t>
+  </si>
+  <si>
+    <t>Dockerizing the Backend/start creation of API's</t>
+  </si>
+  <si>
+    <t>Decided to proceed with AWS.</t>
+  </si>
+  <si>
+    <t>Learning Tech stack( React, Spring, MongoDB)</t>
+  </si>
+  <si>
+    <t>Decided the total Pages required for the work</t>
+  </si>
+  <si>
     <t>1. Feedback</t>
   </si>
   <si>
-    <t>2. Comunication</t>
-  </si>
-  <si>
-    <t>3. Respect</t>
-  </si>
-  <si>
-    <t>WEEK 2 ( MARCH 6 - MARCH 12)</t>
-  </si>
-  <si>
-    <t>Was the scrum master for this sprint. Meanwhile also worked on the frontend decisions along with the tables</t>
-  </si>
-  <si>
-    <t>Finalized the table structure for the Database</t>
-  </si>
-  <si>
-    <t>Dockerizing the Backend/start creation of API's</t>
-  </si>
-  <si>
-    <t>Decided to proceed with AWS.</t>
-  </si>
-  <si>
-    <t>Learning Tech stack( React, Spring, MongoDB)</t>
-  </si>
-  <si>
-    <t>Decided the total Pages required for the work</t>
+    <t>We took feedback for our work and also provided what we felt about others work.</t>
+  </si>
+  <si>
+    <t>We followed Communication during this Scrum since it is necessary to keep every team member upto date about the work</t>
   </si>
   <si>
     <t>WEEK 3 ( MARCH 13 - MARCH 19)</t>
@@ -172,6 +187,15 @@
     <t>Create dummy data in JSON format</t>
   </si>
   <si>
+    <t>3. Courage</t>
+  </si>
+  <si>
+    <t>Courage to ask for more time and keep the work on time</t>
+  </si>
+  <si>
+    <t>4. Respect</t>
+  </si>
+  <si>
     <t>WEEK 5 ( MARCH 27 - APRIL 2)</t>
   </si>
   <si>
@@ -277,35 +301,44 @@
     <t>CSS for the purchase history done</t>
   </si>
   <si>
+    <t>Create a component diagram and architecture diagram</t>
+  </si>
+  <si>
+    <t>1. Comunication</t>
+  </si>
+  <si>
+    <t>2. Respect</t>
+  </si>
+  <si>
+    <t>WEEK 9 ( APRIL 24 - APRIL 30)</t>
+  </si>
+  <si>
+    <t>Backend deployment on cloud</t>
+  </si>
+  <si>
+    <t>Validate integration with frontend and modification to api's</t>
+  </si>
+  <si>
+    <t>Frontend deployment on cloud</t>
+  </si>
+  <si>
     <t>Create class diagram and architecture diagram</t>
   </si>
   <si>
-    <t>WEEK 9 ( APRIL 24 - APRIL 30)</t>
-  </si>
-  <si>
-    <t>Backend deployment on cloud</t>
-  </si>
-  <si>
-    <t>Validate integration with frontend and modification to api's</t>
-  </si>
-  <si>
-    <t>Frontend deployment on cloud</t>
-  </si>
-  <si>
     <t>WEEK 10 ( MAY 1 - MAY 12)</t>
-  </si>
-  <si>
-    <t>Create a component diagram and architecture diagram</t>
-  </si>
-  <si>
-    <t>Design frontent booking route component</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+  </numFmts>
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -313,16 +346,346 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -410,13 +773,255 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -444,18 +1049,68 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
+    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
+    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
+    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
+    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
+    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
+    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
+    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
+    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
+    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
+    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Accent2" xfId="16" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="17" builtinId="31"/>
+    <cellStyle name="20% - Accent1" xfId="18" builtinId="30"/>
+    <cellStyle name="Accent1" xfId="19" builtinId="29"/>
+    <cellStyle name="Neutral" xfId="20" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32"/>
+    <cellStyle name="Bad" xfId="22" builtinId="27"/>
+    <cellStyle name="20% - Accent4" xfId="23" builtinId="42"/>
+    <cellStyle name="Total" xfId="24" builtinId="25"/>
+    <cellStyle name="Output" xfId="25" builtinId="21"/>
+    <cellStyle name="Currency" xfId="26" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38"/>
+    <cellStyle name="Note" xfId="28" builtinId="10"/>
+    <cellStyle name="Input" xfId="29" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="30" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="31" builtinId="22"/>
+    <cellStyle name="Good" xfId="32" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="33" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="34" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="35" builtinId="16"/>
+    <cellStyle name="Comma [0]" xfId="36" builtinId="6"/>
+    <cellStyle name="20% - Accent6" xfId="37" builtinId="50"/>
+    <cellStyle name="Title" xfId="38" builtinId="15"/>
+    <cellStyle name="Currency [0]" xfId="39" builtinId="7"/>
+    <cellStyle name="Warning Text" xfId="40" builtinId="11"/>
+    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9"/>
+    <cellStyle name="20% - Accent2" xfId="42" builtinId="34"/>
+    <cellStyle name="Link" xfId="43" builtinId="8"/>
+    <cellStyle name="Heading 2" xfId="44" builtinId="17"/>
+    <cellStyle name="Comma" xfId="45" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="46" builtinId="23"/>
+    <cellStyle name="60% - Accent3" xfId="47" builtinId="40"/>
+    <cellStyle name="Percent" xfId="48" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -713,27 +1368,27 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
   <dimension ref="A1:D178"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" topLeftCell="A166" workbookViewId="0">
+      <selection activeCell="A182" sqref="A182"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="41.6640625" customWidth="1"/>
-    <col min="2" max="2" width="82" customWidth="1"/>
+    <col min="2" max="2" width="94.5859375" customWidth="1"/>
     <col min="3" max="3" width="74.1640625" customWidth="1"/>
     <col min="4" max="4" width="21.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -741,21 +1396,21 @@
       <c r="C1" s="2"/>
       <c r="D1" s="3"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" s="4"/>
       <c r="D2" s="5"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="5"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" s="4"/>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
@@ -769,7 +1424,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4">
       <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
@@ -783,7 +1438,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4">
       <c r="A7" s="4" t="s">
         <v>10</v>
       </c>
@@ -797,7 +1452,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4">
       <c r="A8" s="4" t="s">
         <v>13</v>
       </c>
@@ -811,7 +1466,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4">
       <c r="A9" s="4" t="s">
         <v>16</v>
       </c>
@@ -825,69 +1480,77 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4">
       <c r="A10" s="4"/>
       <c r="D10" s="5"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4">
       <c r="A11" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D11" s="5"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4">
       <c r="A12" s="4"/>
       <c r="D12" s="5"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4">
       <c r="A13" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D13" s="5"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4">
       <c r="A14" s="4" t="s">
         <v>21</v>
       </c>
+      <c r="B14" t="s">
+        <v>22</v>
+      </c>
       <c r="D14" s="5"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4">
       <c r="A15" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
+      </c>
+      <c r="B15" t="s">
+        <v>24</v>
       </c>
       <c r="D15" s="5"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4">
       <c r="A16" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" s="7"/>
+        <v>25</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="C16" s="7"/>
       <c r="D16" s="8"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4">
       <c r="A19" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="3"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4">
       <c r="A20" s="4"/>
       <c r="D20" s="5"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4">
       <c r="A21" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D21" s="5"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4">
       <c r="A22" s="4"/>
       <c r="D22" s="5"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4">
       <c r="A23" s="4" t="s">
         <v>2</v>
       </c>
@@ -901,125 +1564,133 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4">
       <c r="A24" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B24" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C24" t="s">
-        <v>92</v>
+        <v>29</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4">
       <c r="A25" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B25" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C25" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4">
       <c r="A26" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B26" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C26" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4">
       <c r="A27" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B27" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C27" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4">
       <c r="A28" s="4"/>
       <c r="D28" s="5"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4">
       <c r="A29" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="5"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4">
       <c r="A30" s="4"/>
       <c r="D30" s="5"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4">
       <c r="A31" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D31" s="5"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4">
       <c r="A32" s="4" t="s">
-        <v>21</v>
+        <v>35</v>
+      </c>
+      <c r="B32" t="s">
+        <v>36</v>
       </c>
       <c r="D32" s="5"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4">
       <c r="A33" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
+      </c>
+      <c r="B33" t="s">
+        <v>37</v>
       </c>
       <c r="D33" s="5"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4">
       <c r="A34" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B34" s="7"/>
+        <v>25</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="C34" s="7"/>
       <c r="D34" s="8"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4">
       <c r="A37" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="3"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4">
       <c r="A38" s="4"/>
       <c r="D38" s="5"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4">
       <c r="A39" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D39" s="5"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4">
       <c r="A40" s="4"/>
       <c r="D40" s="5"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4">
       <c r="A41" s="4" t="s">
         <v>2</v>
       </c>
@@ -1033,125 +1704,133 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4">
       <c r="A42" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B42" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C42" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="D42" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4">
       <c r="A43" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B43" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="C43" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="D43" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4">
       <c r="A44" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B44" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="C44" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="D44" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4">
       <c r="A45" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B45" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="C45" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="D45" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4">
       <c r="A46" s="4"/>
       <c r="D46" s="5"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4">
       <c r="A47" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D47" s="5"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4">
       <c r="A48" s="4"/>
       <c r="D48" s="5"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4">
       <c r="A49" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D49" s="5"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4">
       <c r="A50" s="4" t="s">
-        <v>21</v>
+        <v>35</v>
+      </c>
+      <c r="B50" t="s">
+        <v>36</v>
       </c>
       <c r="D50" s="5"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4">
       <c r="A51" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
+      </c>
+      <c r="B51" t="s">
+        <v>37</v>
       </c>
       <c r="D51" s="5"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4">
       <c r="A52" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B52" s="7"/>
+        <v>25</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="C52" s="7"/>
       <c r="D52" s="8"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4">
       <c r="A55" s="1" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
       <c r="D55" s="3"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4">
       <c r="A56" s="4"/>
       <c r="D56" s="5"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4">
       <c r="A57" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D57" s="5"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4">
       <c r="A58" s="4"/>
       <c r="D58" s="5"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4">
       <c r="A59" s="4" t="s">
         <v>2</v>
       </c>
@@ -1165,257 +1844,273 @@
         <v>5</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4">
       <c r="A60" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B60" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="C60" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
       <c r="A61" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B61" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="C61" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="D61" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4">
       <c r="A62" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B62" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="C62" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="D62" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4">
       <c r="A63" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B63" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="C63" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="D63" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4">
       <c r="A64" s="4"/>
       <c r="D64" s="5"/>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4">
       <c r="A65" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D65" s="5"/>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4">
       <c r="A66" s="4"/>
       <c r="D66" s="5"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4">
       <c r="A67" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D67" s="5"/>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:4">
       <c r="A68" s="4" t="s">
-        <v>21</v>
+        <v>35</v>
+      </c>
+      <c r="B68" t="s">
+        <v>36</v>
       </c>
       <c r="D68" s="5"/>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:4">
       <c r="A69" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
+      </c>
+      <c r="B69" t="s">
+        <v>37</v>
       </c>
       <c r="D69" s="5"/>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70" s="6" t="s">
+    <row r="70" spans="1:4">
+      <c r="A70" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B70" t="s">
+        <v>58</v>
+      </c>
+      <c r="D70" s="10"/>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B71" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C71" s="7"/>
+      <c r="D71" s="8"/>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B74" s="2"/>
+      <c r="C74" s="2"/>
+      <c r="D74" s="3"/>
+    </row>
+    <row r="75" spans="1:4">
+      <c r="A75" s="4"/>
+      <c r="D75" s="5"/>
+    </row>
+    <row r="76" spans="1:4">
+      <c r="A76" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D76" s="5"/>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77" s="4"/>
+      <c r="D77" s="5"/>
+    </row>
+    <row r="78" spans="1:4">
+      <c r="A78" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B78" t="s">
+        <v>3</v>
+      </c>
+      <c r="C78" t="s">
+        <v>4</v>
+      </c>
+      <c r="D78" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B79" t="s">
+        <v>61</v>
+      </c>
+      <c r="C79" t="s">
+        <v>62</v>
+      </c>
+      <c r="D79" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="A80" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B80" t="s">
+        <v>63</v>
+      </c>
+      <c r="C80" t="s">
+        <v>64</v>
+      </c>
+      <c r="D80" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="A81" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B81" t="s">
+        <v>65</v>
+      </c>
+      <c r="C81" t="s">
+        <v>66</v>
+      </c>
+      <c r="D81" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
+      <c r="A82" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B82" t="s">
+        <v>67</v>
+      </c>
+      <c r="C82" t="s">
+        <v>68</v>
+      </c>
+      <c r="D82" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
+      <c r="A83" s="4"/>
+      <c r="D83" s="5"/>
+    </row>
+    <row r="84" spans="1:4">
+      <c r="A84" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D84" s="5"/>
+    </row>
+    <row r="85" spans="1:4">
+      <c r="A85" s="4"/>
+      <c r="D85" s="5"/>
+    </row>
+    <row r="86" spans="1:4">
+      <c r="A86" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D86" s="5"/>
+    </row>
+    <row r="87" spans="1:4">
+      <c r="A87" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B87" t="s">
+        <v>36</v>
+      </c>
+      <c r="D87" s="5"/>
+    </row>
+    <row r="88" spans="1:4">
+      <c r="A88" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B70" s="7"/>
-      <c r="C70" s="7"/>
-      <c r="D70" s="8"/>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B73" s="2"/>
-      <c r="C73" s="2"/>
-      <c r="D73" s="3"/>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74" s="4"/>
-      <c r="D74" s="5"/>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A75" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D75" s="5"/>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A76" s="4"/>
-      <c r="D76" s="5"/>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A77" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B77" t="s">
-        <v>3</v>
-      </c>
-      <c r="C77" t="s">
-        <v>4</v>
-      </c>
-      <c r="D77" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A78" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B78" t="s">
-        <v>51</v>
-      </c>
-      <c r="C78" t="s">
-        <v>52</v>
-      </c>
-      <c r="D78" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A79" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B79" t="s">
-        <v>53</v>
-      </c>
-      <c r="C79" t="s">
-        <v>54</v>
-      </c>
-      <c r="D79" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A80" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B80" t="s">
-        <v>55</v>
-      </c>
-      <c r="C80" t="s">
-        <v>56</v>
-      </c>
-      <c r="D80" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A81" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B81" t="s">
-        <v>57</v>
-      </c>
-      <c r="C81" t="s">
-        <v>58</v>
-      </c>
-      <c r="D81" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A82" s="4"/>
-      <c r="D82" s="5"/>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A83" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D83" s="5"/>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A84" s="4"/>
-      <c r="D84" s="5"/>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A85" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D85" s="5"/>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A86" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D86" s="5"/>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A87" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D87" s="5"/>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A88" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B88" s="7"/>
-      <c r="C88" s="7"/>
-      <c r="D88" s="8"/>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B88" t="s">
+        <v>37</v>
+      </c>
+      <c r="C88"/>
+      <c r="D88" s="5"/>
+    </row>
+    <row r="91" spans="1:4">
       <c r="A91" s="1" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
       <c r="D91" s="3"/>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:4">
       <c r="A92" s="4"/>
       <c r="D92" s="5"/>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:4">
       <c r="A93" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D93" s="5"/>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:4">
       <c r="A94" s="4"/>
       <c r="D94" s="5"/>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:4">
       <c r="A95" s="4" t="s">
         <v>2</v>
       </c>
@@ -1429,125 +2124,133 @@
         <v>5</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:4">
       <c r="A96" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B96" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="C96" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="D96" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:4">
       <c r="A97" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B97" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="C97" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="D97" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:4">
       <c r="A98" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B98" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="C98" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="D98" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:4">
       <c r="A99" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B99" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="C99" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="D99" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:4">
       <c r="A100" s="4"/>
       <c r="D100" s="5"/>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:4">
       <c r="A101" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D101" s="5"/>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:4">
       <c r="A102" s="4"/>
       <c r="D102" s="5"/>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:4">
       <c r="A103" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D103" s="5"/>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:4">
       <c r="A104" s="4" t="s">
-        <v>21</v>
+        <v>35</v>
+      </c>
+      <c r="B104" t="s">
+        <v>36</v>
       </c>
       <c r="D104" s="5"/>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:4">
       <c r="A105" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
+      </c>
+      <c r="B105" t="s">
+        <v>37</v>
       </c>
       <c r="D105" s="5"/>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:4">
       <c r="A106" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B106" s="7"/>
+        <v>25</v>
+      </c>
+      <c r="B106" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="C106" s="7"/>
       <c r="D106" s="8"/>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:4">
       <c r="A109" s="1" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="B109" s="2"/>
       <c r="C109" s="2"/>
       <c r="D109" s="3"/>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:4">
       <c r="A110" s="4"/>
       <c r="D110" s="5"/>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:4">
       <c r="A111" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D111" s="5"/>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:4">
       <c r="A112" s="4"/>
       <c r="D112" s="5"/>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:4">
       <c r="A113" s="4" t="s">
         <v>2</v>
       </c>
@@ -1561,257 +2264,274 @@
         <v>5</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:4">
       <c r="A114" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B114" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="C114" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="D114" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:4">
       <c r="A115" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B115" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="C115" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="D115" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:4">
       <c r="A116" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B116" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="C116" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="D116" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:4">
       <c r="A117" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B117" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="C117" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="D117" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:4">
       <c r="A118" s="4"/>
       <c r="D118" s="5"/>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:4">
       <c r="A119" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D119" s="5"/>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:4">
       <c r="A120" s="4"/>
       <c r="D120" s="5"/>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:4">
       <c r="A121" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D121" s="5"/>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:4">
       <c r="A122" s="4" t="s">
-        <v>21</v>
+        <v>35</v>
+      </c>
+      <c r="B122" t="s">
+        <v>36</v>
       </c>
       <c r="D122" s="5"/>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:4">
       <c r="A123" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
+      </c>
+      <c r="B123" t="s">
+        <v>37</v>
       </c>
       <c r="D123" s="5"/>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A124" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B124" s="7"/>
-      <c r="C124" s="7"/>
-      <c r="D124" s="8"/>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A127" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B127" s="2"/>
-      <c r="C127" s="2"/>
-      <c r="D127" s="3"/>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A128" s="4"/>
-      <c r="D128" s="5"/>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A129" s="4" t="s">
+    <row r="124" spans="1:4">
+      <c r="A124" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B124" t="s">
+        <v>58</v>
+      </c>
+      <c r="C124"/>
+      <c r="D124" s="10"/>
+    </row>
+    <row r="125" spans="1:4">
+      <c r="A125" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B125" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C125" s="7"/>
+      <c r="D125" s="8"/>
+    </row>
+    <row r="128" spans="1:4">
+      <c r="A128" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B128" s="2"/>
+      <c r="C128" s="2"/>
+      <c r="D128" s="3"/>
+    </row>
+    <row r="129" spans="1:4">
+      <c r="A129" s="4"/>
+      <c r="D129" s="5"/>
+    </row>
+    <row r="130" spans="1:4">
+      <c r="A130" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D129" s="5"/>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A130" s="4"/>
       <c r="D130" s="5"/>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A131" s="4" t="s">
+    <row r="131" spans="1:4">
+      <c r="A131" s="4"/>
+      <c r="D131" s="5"/>
+    </row>
+    <row r="132" spans="1:4">
+      <c r="A132" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B131" t="s">
+      <c r="B132" t="s">
         <v>3</v>
       </c>
-      <c r="C131" t="s">
+      <c r="C132" t="s">
         <v>4</v>
       </c>
-      <c r="D131" s="5" t="s">
+      <c r="D132" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A132" s="4" t="s">
+    <row r="133" spans="1:4">
+      <c r="A133" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B132" t="s">
-        <v>78</v>
-      </c>
-      <c r="C132" t="s">
-        <v>79</v>
-      </c>
-      <c r="D132" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A133" s="4" t="s">
+      <c r="B133" t="s">
+        <v>88</v>
+      </c>
+      <c r="C133" t="s">
+        <v>89</v>
+      </c>
+      <c r="D133" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4">
+      <c r="A134" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B133" t="s">
-        <v>80</v>
-      </c>
-      <c r="C133" t="s">
-        <v>81</v>
-      </c>
-      <c r="D133" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A134" s="4" t="s">
+      <c r="B134" t="s">
+        <v>90</v>
+      </c>
+      <c r="C134" t="s">
+        <v>91</v>
+      </c>
+      <c r="D134" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4">
+      <c r="A135" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B134" t="s">
-        <v>82</v>
-      </c>
-      <c r="C134" t="s">
-        <v>83</v>
-      </c>
-      <c r="D134" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A135" s="4" t="s">
+      <c r="B135" t="s">
+        <v>92</v>
+      </c>
+      <c r="C135" t="s">
+        <v>93</v>
+      </c>
+      <c r="D135" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4">
+      <c r="A136" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B135" t="s">
-        <v>84</v>
-      </c>
-      <c r="C135" t="s">
-        <v>91</v>
-      </c>
-      <c r="D135" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A136" s="4"/>
-      <c r="D136" s="5"/>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A137" s="4" t="s">
+      <c r="B136" t="s">
+        <v>94</v>
+      </c>
+      <c r="C136" t="s">
+        <v>95</v>
+      </c>
+      <c r="D136" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4">
+      <c r="A137" s="4"/>
+      <c r="D137" s="5"/>
+    </row>
+    <row r="138" spans="1:4">
+      <c r="A138" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D137" s="5"/>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A138" s="4"/>
       <c r="D138" s="5"/>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A139" s="4" t="s">
+    <row r="139" spans="1:4">
+      <c r="A139" s="4"/>
+      <c r="D139" s="5"/>
+    </row>
+    <row r="140" spans="1:4">
+      <c r="A140" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D139" s="5"/>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A140" s="4" t="s">
-        <v>21</v>
-      </c>
       <c r="D140" s="5"/>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:4">
       <c r="A141" s="4" t="s">
-        <v>22</v>
+        <v>96</v>
+      </c>
+      <c r="B141" t="s">
+        <v>37</v>
       </c>
       <c r="D141" s="5"/>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:4">
       <c r="A142" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B142" s="7"/>
+        <v>97</v>
+      </c>
+      <c r="B142" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="C142" s="7"/>
       <c r="D142" s="8"/>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:4">
       <c r="A145" s="1" t="s">
-        <v>86</v>
+        <v>98</v>
       </c>
       <c r="B145" s="2"/>
       <c r="C145" s="2"/>
       <c r="D145" s="3"/>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:4">
       <c r="A146" s="4"/>
       <c r="D146" s="5"/>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:4">
       <c r="A147" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D147" s="5"/>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:4">
       <c r="A148" s="4"/>
       <c r="D148" s="5"/>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:4">
       <c r="A149" s="4" t="s">
         <v>2</v>
       </c>
@@ -1825,235 +2545,253 @@
         <v>5</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:4">
       <c r="A150" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B150" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="C150" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="D150" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:4">
       <c r="A151" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B151" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="C151" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="D151" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:4">
       <c r="A152" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B152" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="C152" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="D152" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:4">
       <c r="A153" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B153" t="s">
-        <v>85</v>
+        <v>102</v>
       </c>
       <c r="C153" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="D153" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:4">
       <c r="A154" s="4"/>
       <c r="D154" s="5"/>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:4">
       <c r="A155" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D155" s="5"/>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:4">
       <c r="A156" s="4"/>
       <c r="D156" s="5"/>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:4">
       <c r="A157" s="4" t="s">
         <v>20</v>
       </c>
+      <c r="B157"/>
       <c r="D157" s="5"/>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:4">
       <c r="A158" s="4" t="s">
-        <v>21</v>
+        <v>96</v>
+      </c>
+      <c r="B158" t="s">
+        <v>37</v>
       </c>
       <c r="D158" s="5"/>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A159" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D159" s="5"/>
-    </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A160" s="6" t="s">
+    <row r="159" spans="1:4">
+      <c r="A159" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B159" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C159" s="7"/>
+      <c r="D159" s="8"/>
+    </row>
+    <row r="162" spans="1:4">
+      <c r="A162" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B162" s="2"/>
+      <c r="C162" s="2"/>
+      <c r="D162" s="3"/>
+    </row>
+    <row r="163" spans="1:4">
+      <c r="A163" s="4"/>
+      <c r="D163" s="5"/>
+    </row>
+    <row r="164" spans="1:4">
+      <c r="A164" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D164" s="5"/>
+    </row>
+    <row r="165" spans="1:4">
+      <c r="A165" s="4"/>
+      <c r="D165" s="5"/>
+    </row>
+    <row r="166" spans="1:4">
+      <c r="A166" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B166" t="s">
+        <v>3</v>
+      </c>
+      <c r="C166" t="s">
+        <v>4</v>
+      </c>
+      <c r="D166" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4">
+      <c r="A167" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B167" t="s">
+        <v>89</v>
+      </c>
+      <c r="C167" t="s">
+        <v>99</v>
+      </c>
+      <c r="D167" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4">
+      <c r="A168" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B168" t="s">
+        <v>100</v>
+      </c>
+      <c r="C168" t="s">
+        <v>99</v>
+      </c>
+      <c r="D168" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4">
+      <c r="A169" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B169" t="s">
+        <v>93</v>
+      </c>
+      <c r="C169" t="s">
+        <v>101</v>
+      </c>
+      <c r="D169" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4">
+      <c r="A170" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B170" t="s">
+        <v>102</v>
+      </c>
+      <c r="C170" t="s">
+        <v>101</v>
+      </c>
+      <c r="D170" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4">
+      <c r="A171" s="4"/>
+      <c r="D171" s="5"/>
+    </row>
+    <row r="172" spans="1:4">
+      <c r="A172" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D172" s="5"/>
+    </row>
+    <row r="173" spans="1:4">
+      <c r="A173" s="4"/>
+      <c r="D173" s="5"/>
+    </row>
+    <row r="174" spans="1:4">
+      <c r="A174" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D174" s="5"/>
+    </row>
+    <row r="175" spans="1:4">
+      <c r="A175" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B175" t="s">
+        <v>36</v>
+      </c>
+      <c r="D175" s="5"/>
+    </row>
+    <row r="176" spans="1:4">
+      <c r="A176" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B160" s="7"/>
-      <c r="C160" s="7"/>
-      <c r="D160" s="8"/>
-    </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A163" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B163" s="2"/>
-      <c r="C163" s="2"/>
-      <c r="D163" s="3"/>
-    </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A164" s="4"/>
-      <c r="D164" s="5"/>
-    </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A165" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D165" s="5"/>
-    </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A166" s="4"/>
-      <c r="D166" s="5"/>
-    </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A167" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B167" t="s">
-        <v>3</v>
-      </c>
-      <c r="C167" t="s">
-        <v>4</v>
-      </c>
-      <c r="D167" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A168" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B168" t="s">
-        <v>79</v>
-      </c>
-      <c r="C168" t="s">
-        <v>87</v>
-      </c>
-      <c r="D168" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A169" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B169" t="s">
-        <v>88</v>
-      </c>
-      <c r="C169" t="s">
-        <v>87</v>
-      </c>
-      <c r="D169" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A170" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B170" t="s">
-        <v>83</v>
-      </c>
-      <c r="C170" t="s">
-        <v>89</v>
-      </c>
-      <c r="D170" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A171" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B171" t="s">
-        <v>85</v>
-      </c>
-      <c r="C171" t="s">
-        <v>89</v>
-      </c>
-      <c r="D171" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A172" s="4"/>
-      <c r="D172" s="5"/>
-    </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A173" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D173" s="5"/>
-    </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A174" s="4"/>
-      <c r="D174" s="5"/>
-    </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A175" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D175" s="5"/>
-    </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A176" s="4" t="s">
-        <v>21</v>
+      <c r="B176" t="s">
+        <v>37</v>
       </c>
       <c r="D176" s="5"/>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A177" s="4" t="s">
-        <v>22</v>
+    <row r="177" spans="1:4">
+      <c r="A177" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B177" t="s">
+        <v>58</v>
       </c>
       <c r="D177" s="5"/>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:4">
       <c r="A178" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B178" s="7"/>
+        <v>59</v>
+      </c>
+      <c r="B178" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="C178" s="7"/>
       <c r="D178" s="8"/>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>